<commit_message>
Fixing Accuracy of Model
</commit_message>
<xml_diff>
--- a/Data/ThermalDiffusivity.xlsx
+++ b/Data/ThermalDiffusivity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christopher\Desktop\APPM 4350\APPM-4350-Cooling-Sphere\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C64A11D6-7184-4C89-9E07-E0F685FA72E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C103038-1380-4615-A8B6-7CD35623A362}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8" yWindow="8" windowWidth="20505" windowHeight="12945" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6105" yWindow="2453" windowWidth="20505" windowHeight="12944" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Material</t>
   </si>
@@ -63,6 +63,15 @@
   </si>
   <si>
     <t>Steel, Chrome-Nuckel, 18%cr-8%Ni</t>
+  </si>
+  <si>
+    <t>Steel, Stainless, 316</t>
+  </si>
+  <si>
+    <t>https://www.engineersedge.com/properties_of_metals.htm#:~:text=Thermal%20Properties%20of%20Metals%2C%20Conductivity%2C%20Thermal%20Expansion%2C%20Specific%20Heat,-Heat%20Transfer%20Engineering&amp;text=Metals%20in%20general%20have%20high,metals%20are%20shiny%20and%20lustrous</t>
+  </si>
+  <si>
+    <t>Steel, Chrome, Cr5%</t>
   </si>
 </sst>
 </file>
@@ -392,10 +401,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -407,7 +416,7 @@
     <col min="5" max="5" width="15.46484375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -424,7 +433,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -443,7 +452,7 @@
         <v>2.0451364414177671E-5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -458,11 +467,11 @@
         <v>460</v>
       </c>
       <c r="E3" s="2">
-        <f t="shared" ref="E3:E6" si="0">B3/(C3*D3)</f>
+        <f t="shared" ref="E3:E7" si="0">B3/(C3*D3)</f>
         <v>1.6860609745985241E-5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -481,9 +490,9 @@
         <v>6.2200659326988865E-6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B5">
         <v>40</v>
@@ -500,7 +509,7 @@
         <v>1.110130495839786E-5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -515,7 +524,32 @@
         <v>460</v>
       </c>
       <c r="E6" s="2">
+        <f t="shared" si="0"/>
         <v>4.5330411422151277E-6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>16.260000000000002</v>
+      </c>
+      <c r="C7">
+        <f>8.0272 * POWER(10,3)</f>
+        <v>8027.2000000000007</v>
+      </c>
+      <c r="D7">
+        <v>502.1</v>
+      </c>
+      <c r="E7" s="2">
+        <f t="shared" si="0"/>
+        <v>4.0342818484073092E-6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="F10" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.45">

</xml_diff>